<commit_message>
what-if analysis with 2 variables:: by sergio giraldo @ 20230309T1112CET, gpg signed
</commit_message>
<xml_diff>
--- a/excel/pivot-table.xlsx
+++ b/excel/pivot-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GK47LX/source/office/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FB8A8D-0FA7-FF4A-99D0-B3EDABD71E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152F1769-146F-C04C-B730-C57F6869A126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="-9620" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SalesOrders" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
     <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="50">
   <si>
     <t>Region</t>
   </si>
@@ -154,9 +154,6 @@
     <t>3. choose what goes in rows, what goes in columns</t>
   </si>
   <si>
-    <t>4. the columns are the aggregations, compare the 2 pivot on the left. Top is the count of items per region summarized by item; bottom is also the count of items per region but summarized by region. Same numbers but from different angles</t>
-  </si>
-  <si>
     <t>5. you can choose the fields clicking on the upper cell on the pivot table to bring the menu. Then choose 'Field list'</t>
   </si>
   <si>
@@ -182,6 +179,15 @@
   </si>
   <si>
     <t>For this, select the PivotTable, menu Pivot Table Analyze-&gt;Options-&gt;Show Report Filter Pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. the columns are the aggregations, compare the 2 pivot on the left. Top is the count of items per region </t>
+  </si>
+  <si>
+    <t xml:space="preserve">summarized by item; bottom is also the count of items per region but summarized by region. </t>
+  </si>
+  <si>
+    <t>Same numbers but from different angles</t>
   </si>
 </sst>
 </file>
@@ -387,7 +393,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -428,30 +434,27 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" pivotButton="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -461,9 +464,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -472,7 +475,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 4" xfId="3" xr:uid="{1A867160-CFF8-4CFB-9486-A3FC92514B8F}"/>
   </cellStyles>
-  <dxfs count="148">
+  <dxfs count="165">
     <dxf>
       <font>
         <sz val="14"/>
@@ -510,7 +513,427 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="9"/>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
       </font>
     </dxf>
     <dxf>
@@ -676,26 +1099,54 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -759,276 +1210,6 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <sz val="14"/>
       </font>
     </dxf>
@@ -1215,116 +1396,6 @@
     <dxf>
       <font>
         <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Times New Roman"/>
-        <family val="1"/>
       </font>
     </dxf>
     <dxf>
@@ -2541,7 +2612,664 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{07408818-21B1-604D-97DE-6F57DD48BBD6}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{053A0F0D-0B52-5E4B-8BFD-D3ADFE2F322B}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="J27:K33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="7">
+    <pivotField compact="0" numFmtId="165" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="44">
+        <item x="0"/>
+        <item x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item h="1" x="4"/>
+        <item h="1" x="5"/>
+        <item h="1" x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="8"/>
+        <item h="1" x="9"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item h="1" x="12"/>
+        <item h="1" x="13"/>
+        <item h="1" x="14"/>
+        <item h="1" x="15"/>
+        <item h="1" x="16"/>
+        <item h="1" x="17"/>
+        <item h="1" x="18"/>
+        <item h="1" x="19"/>
+        <item h="1" x="20"/>
+        <item h="1" x="21"/>
+        <item h="1" x="22"/>
+        <item h="1" x="23"/>
+        <item h="1" x="24"/>
+        <item h="1" x="25"/>
+        <item h="1" x="26"/>
+        <item h="1" x="27"/>
+        <item h="1" x="28"/>
+        <item h="1" x="29"/>
+        <item h="1" x="30"/>
+        <item h="1" x="31"/>
+        <item h="1" x="32"/>
+        <item h="1" x="33"/>
+        <item h="1" x="34"/>
+        <item h="1" x="35"/>
+        <item h="1" x="36"/>
+        <item h="1" x="37"/>
+        <item h="1" x="38"/>
+        <item h="1" x="39"/>
+        <item h="1" x="40"/>
+        <item h="1" x="41"/>
+        <item h="1" x="42"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" compact="0" outline="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0">
+      <items count="6">
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0">
+      <items count="42">
+        <item x="34"/>
+        <item x="37"/>
+        <item x="23"/>
+        <item x="38"/>
+        <item x="10"/>
+        <item x="8"/>
+        <item x="27"/>
+        <item x="19"/>
+        <item x="26"/>
+        <item x="40"/>
+        <item x="24"/>
+        <item x="6"/>
+        <item x="35"/>
+        <item x="4"/>
+        <item x="12"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="25"/>
+        <item x="13"/>
+        <item x="15"/>
+        <item x="14"/>
+        <item x="5"/>
+        <item x="17"/>
+        <item x="30"/>
+        <item x="21"/>
+        <item x="7"/>
+        <item x="18"/>
+        <item x="9"/>
+        <item x="3"/>
+        <item x="16"/>
+        <item x="29"/>
+        <item x="31"/>
+        <item x="28"/>
+        <item x="33"/>
+        <item x="1"/>
+        <item x="32"/>
+        <item x="36"/>
+        <item x="20"/>
+        <item x="22"/>
+        <item x="11"/>
+        <item x="39"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Item" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="38">
+    <format dxfId="117">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="116">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="115">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="114">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
+    </format>
+    <format dxfId="113">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="112">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="111">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="2">
+            <x v="0"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="110">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="109">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="108">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="107">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="106">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="105">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="104">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
+    </format>
+    <format dxfId="103">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="102">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="101">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="2">
+            <x v="0"/>
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="100">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="99">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="2">
+            <x v="0"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="98">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="97">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="96">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="95">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="94">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="93">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="92">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="91">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="90">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="89">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="88">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="87">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="86">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="85">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="84">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="83">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="82">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="81">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="80">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight14" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{960F1C2F-DFA5-6843-BD55-C3FCFFA11A4D}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A37:B81" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField axis="axisRow" compact="0" numFmtId="165" outline="0" showAll="0">
+      <items count="44">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="44">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Unit Cost" fld="5" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{35B84901-240D-3E41-87ED-BDEEB4967361}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A29:G34" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
+    <pivotField compact="0" numFmtId="165" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisCol" dataField="1" compact="0" outline="0" showAll="0">
+      <items count="6">
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="3"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Item" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="10">
+    <format dxfId="127">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="126">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="125">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="124">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="123">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="122">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="121">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="120">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="119">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="118">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{07408818-21B1-604D-97DE-6F57DD48BBD6}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="3">
   <location ref="A20:E27" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField compact="0" numFmtId="165" outline="0" showAll="0"/>
@@ -2657,42 +3385,42 @@
     <dataField name="Count of Item" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="10">
-    <format dxfId="100">
+    <format dxfId="137">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="99">
+    <format dxfId="136">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="98">
+    <format dxfId="135">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="97">
+    <format dxfId="134">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="96">
+    <format dxfId="133">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="95">
+    <format dxfId="132">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="94">
+    <format dxfId="131">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="93">
+    <format dxfId="130">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="92">
+    <format dxfId="129">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="128">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -2818,7 +3546,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9F05F403-2D44-214F-BB09-91E3814404E5}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:V18" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="7">
@@ -3027,45 +3755,45 @@
     <dataField name="Sum of Total" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="18">
-    <format dxfId="118">
+    <format dxfId="155">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="117">
+    <format dxfId="154">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="116">
+    <format dxfId="153">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="115">
+    <format dxfId="152">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="114">
+    <format dxfId="151">
       <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="113">
+    <format dxfId="150">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="112">
+    <format dxfId="149">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="111">
+    <format dxfId="148">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="110">
+    <format dxfId="147">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="109">
+    <format dxfId="146">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="108">
+    <format dxfId="145">
       <pivotArea field="3" dataOnly="0" labelOnly="1" grandCol="1" outline="0" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -3074,7 +3802,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="107">
+    <format dxfId="144">
       <pivotArea field="3" dataOnly="0" labelOnly="1" grandCol="1" outline="0" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -3083,7 +3811,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="106">
+    <format dxfId="143">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="2">
@@ -3096,7 +3824,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="105">
+    <format dxfId="142">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="2">
@@ -3109,7 +3837,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="104">
+    <format dxfId="141">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="2">
@@ -3122,7 +3850,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="103">
+    <format dxfId="140">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="2">
@@ -3135,7 +3863,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="102">
+    <format dxfId="139">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="2">
@@ -3148,7 +3876,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="101">
+    <format dxfId="138">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="2">
@@ -3160,663 +3888,6 @@
           </reference>
         </references>
       </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{053A0F0D-0B52-5E4B-8BFD-D3ADFE2F322B}" name="PivotTable4" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="J27:K33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="7">
-    <pivotField compact="0" numFmtId="165" outline="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="44">
-        <item x="0"/>
-        <item x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item h="1" x="4"/>
-        <item h="1" x="5"/>
-        <item h="1" x="6"/>
-        <item h="1" x="7"/>
-        <item h="1" x="8"/>
-        <item h="1" x="9"/>
-        <item h="1" x="10"/>
-        <item h="1" x="11"/>
-        <item h="1" x="12"/>
-        <item h="1" x="13"/>
-        <item h="1" x="14"/>
-        <item h="1" x="15"/>
-        <item h="1" x="16"/>
-        <item h="1" x="17"/>
-        <item h="1" x="18"/>
-        <item h="1" x="19"/>
-        <item h="1" x="20"/>
-        <item h="1" x="21"/>
-        <item h="1" x="22"/>
-        <item h="1" x="23"/>
-        <item h="1" x="24"/>
-        <item h="1" x="25"/>
-        <item h="1" x="26"/>
-        <item h="1" x="27"/>
-        <item h="1" x="28"/>
-        <item h="1" x="29"/>
-        <item h="1" x="30"/>
-        <item h="1" x="31"/>
-        <item h="1" x="32"/>
-        <item h="1" x="33"/>
-        <item h="1" x="34"/>
-        <item h="1" x="35"/>
-        <item h="1" x="36"/>
-        <item h="1" x="37"/>
-        <item h="1" x="38"/>
-        <item h="1" x="39"/>
-        <item h="1" x="40"/>
-        <item h="1" x="41"/>
-        <item h="1" x="42"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" compact="0" outline="0" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0">
-      <items count="6">
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" outline="0" showAll="0">
-      <items count="42">
-        <item x="34"/>
-        <item x="37"/>
-        <item x="23"/>
-        <item x="38"/>
-        <item x="10"/>
-        <item x="8"/>
-        <item x="27"/>
-        <item x="19"/>
-        <item x="26"/>
-        <item x="40"/>
-        <item x="24"/>
-        <item x="6"/>
-        <item x="35"/>
-        <item x="4"/>
-        <item x="12"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="25"/>
-        <item x="13"/>
-        <item x="15"/>
-        <item x="14"/>
-        <item x="5"/>
-        <item x="17"/>
-        <item x="30"/>
-        <item x="21"/>
-        <item x="7"/>
-        <item x="18"/>
-        <item x="9"/>
-        <item x="3"/>
-        <item x="16"/>
-        <item x="29"/>
-        <item x="31"/>
-        <item x="28"/>
-        <item x="33"/>
-        <item x="1"/>
-        <item x="32"/>
-        <item x="36"/>
-        <item x="20"/>
-        <item x="22"/>
-        <item x="11"/>
-        <item x="39"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count of Item" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="38">
-    <format dxfId="138">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="137">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="136">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="135">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
-    </format>
-    <format dxfId="134">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="133">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="132">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="2">
-            <x v="0"/>
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="131">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="130">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="2">
-            <x v="0"/>
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="129">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="128">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="127">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="126">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="125">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
-    </format>
-    <format dxfId="124">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="123">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="122">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="2">
-            <x v="0"/>
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="121">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="120">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="2">
-            <x v="0"/>
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="119">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="20">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="19">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="18">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="17">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="16">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="15">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="13">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="12">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="11">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="10">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="9">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="8">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="6">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="5">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="4">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="3">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="2">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="1">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight14" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{960F1C2F-DFA5-6843-BD55-C3FCFFA11A4D}" name="PivotTable5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A37:B81" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField axis="axisRow" compact="0" numFmtId="165" outline="0" showAll="0">
-      <items count="44">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="36"/>
-        <item x="37"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="41"/>
-        <item x="42"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="44">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="39"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Unit Cost" fld="5" baseField="0" baseItem="0" numFmtId="164"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{35B84901-240D-3E41-87ED-BDEEB4967361}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="A29:G34" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="7">
-    <pivotField compact="0" numFmtId="165" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisCol" dataField="1" compact="0" outline="0" showAll="0">
-      <items count="6">
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
-    <pivotField compact="0" numFmtId="164" outline="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="3"/>
-  </colFields>
-  <colItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Item" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="10">
-    <format dxfId="81">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="82">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="83">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="84">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="85">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="86">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
-    </format>
-    <format dxfId="87">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="88">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="89">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="90">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -3832,7 +3903,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{053A0F0D-0B52-5E4B-8BFD-D3ADFE2F322B}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{053A0F0D-0B52-5E4B-8BFD-D3ADFE2F322B}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField compact="0" numFmtId="165" outline="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -3984,25 +4055,25 @@
     <dataField name="Count of Item" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="20">
-    <format dxfId="21">
+    <format dxfId="79">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="78">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="77">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="76">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="75">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="74">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="73">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="3" count="2">
@@ -4012,10 +4083,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="72">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="29">
+    <format dxfId="71">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="2">
@@ -4025,28 +4096,28 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="70">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="69">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="68">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="67">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="66">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="65">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="64">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="63">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="3" count="2">
@@ -4056,10 +4127,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="62">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="61">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="2">
@@ -4069,7 +4140,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="60">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -4086,7 +4157,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{053A0F0D-0B52-5E4B-8BFD-D3ADFE2F322B}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{053A0F0D-0B52-5E4B-8BFD-D3ADFE2F322B}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField compact="0" numFmtId="165" outline="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -4235,25 +4306,25 @@
     <dataField name="Count of Item" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="20">
-    <format dxfId="41">
+    <format dxfId="59">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="58">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="57">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="56">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="55">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="54">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="53">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="3" count="2">
@@ -4263,10 +4334,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="52">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="51">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="2">
@@ -4279,25 +4350,25 @@
     <format dxfId="50">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="49">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="48">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="53">
+    <format dxfId="47">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="54">
+    <format dxfId="46">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="55">
+    <format dxfId="45">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="56">
+    <format dxfId="44">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="57">
+    <format dxfId="43">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="3" count="2">
@@ -4307,10 +4378,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="42">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="59">
+    <format dxfId="41">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="2">
@@ -4320,7 +4391,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="40">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -4337,7 +4408,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{053A0F0D-0B52-5E4B-8BFD-D3ADFE2F322B}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{053A0F0D-0B52-5E4B-8BFD-D3ADFE2F322B}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField compact="0" numFmtId="165" outline="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -4486,25 +4557,25 @@
     <dataField name="Count of Item" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="20">
-    <format dxfId="61">
+    <format dxfId="39">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="62">
+    <format dxfId="38">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="63">
+    <format dxfId="37">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="64">
+    <format dxfId="36">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="65">
+    <format dxfId="35">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="66">
+    <format dxfId="34">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="67">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="3" count="2">
@@ -4514,10 +4585,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="69">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="2">
@@ -4527,28 +4598,28 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="71">
+    <format dxfId="29">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="72">
+    <format dxfId="28">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="73">
+    <format dxfId="27">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="74">
+    <format dxfId="26">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="75">
+    <format dxfId="25">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="76">
+    <format dxfId="24">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="77">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="3" count="2">
@@ -4558,10 +4629,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="79">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="2">
@@ -4571,7 +4642,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
@@ -4588,16 +4659,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G44" totalsRowShown="0" headerRowDxfId="147" dataDxfId="146">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G44" totalsRowShown="0" headerRowDxfId="164" dataDxfId="163">
   <autoFilter ref="A1:G44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="OrderDate" dataDxfId="145"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Region" dataDxfId="144"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Rep" dataDxfId="143"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Item" dataDxfId="142"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Units" dataDxfId="141"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Unit Cost" dataDxfId="140"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Total" dataDxfId="139"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="OrderDate" dataDxfId="162"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Region" dataDxfId="161"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Rep" dataDxfId="160"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Item" dataDxfId="159"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Units" dataDxfId="158"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Unit Cost" dataDxfId="157"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Total" dataDxfId="156"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5973,19 +6044,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2DB7D1-11AC-9649-BC92-38E5995EE8C1}">
   <dimension ref="A3:V81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:B26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.33203125" customWidth="1"/>
@@ -6086,7 +6153,7 @@
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
       <c r="Q4" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R4" s="13"/>
       <c r="S4" s="13"/>
@@ -6166,43 +6233,43 @@
       <c r="A6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="13">
         <v>1</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="13">
         <v>28</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="13">
         <v>139.72</v>
       </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18">
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13">
         <v>3</v>
       </c>
-      <c r="O6" s="18">
+      <c r="O6" s="13">
         <v>155</v>
       </c>
-      <c r="P6" s="18">
+      <c r="P6" s="13">
         <v>298.65000000000003</v>
       </c>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18">
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13">
         <v>4</v>
       </c>
-      <c r="U6" s="18">
+      <c r="U6" s="13">
         <v>183</v>
       </c>
-      <c r="V6" s="18">
+      <c r="V6" s="13">
         <v>438.37000000000006</v>
       </c>
     </row>
@@ -6210,49 +6277,49 @@
       <c r="A7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="13">
         <v>2</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="13">
         <v>126</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="13">
         <v>1132.74</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18">
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13">
         <v>1</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="13">
         <v>27</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="13">
         <v>539.7299999999999</v>
       </c>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18">
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13">
         <v>2</v>
       </c>
-      <c r="O7" s="18">
+      <c r="O7" s="13">
         <v>60</v>
       </c>
-      <c r="P7" s="18">
+      <c r="P7" s="13">
         <v>77.400000000000006</v>
       </c>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18">
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13">
         <v>5</v>
       </c>
-      <c r="U7" s="18">
+      <c r="U7" s="13">
         <v>213</v>
       </c>
-      <c r="V7" s="18">
+      <c r="V7" s="13">
         <v>1749.8699999999997</v>
       </c>
     </row>
@@ -6260,43 +6327,43 @@
       <c r="A8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="13">
         <v>1</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="13">
         <v>29</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="13">
         <v>57.71</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18">
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13">
         <v>1</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="13">
         <v>96</v>
       </c>
-      <c r="J8" s="18">
+      <c r="J8" s="13">
         <v>479.04</v>
       </c>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18">
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13">
         <v>2</v>
       </c>
-      <c r="U8" s="18">
+      <c r="U8" s="13">
         <v>125</v>
       </c>
-      <c r="V8" s="18">
+      <c r="V8" s="13">
         <v>536.75</v>
       </c>
     </row>
@@ -6304,49 +6371,49 @@
       <c r="A9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="13">
         <v>2</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="13">
         <v>105</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="13">
         <v>1933.95</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18">
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13">
         <v>1</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="13">
         <v>50</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="13">
         <v>249.5</v>
       </c>
-      <c r="N9" s="18">
+      <c r="N9" s="13">
         <v>2</v>
       </c>
-      <c r="O9" s="18">
+      <c r="O9" s="13">
         <v>126</v>
       </c>
-      <c r="P9" s="18">
+      <c r="P9" s="13">
         <v>628.74</v>
       </c>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18">
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13">
         <v>5</v>
       </c>
-      <c r="U9" s="18">
+      <c r="U9" s="13">
         <v>281</v>
       </c>
-      <c r="V9" s="18">
+      <c r="V9" s="13">
         <v>2812.1899999999996</v>
       </c>
     </row>
@@ -6354,55 +6421,55 @@
       <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="13">
         <v>3</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="13">
         <v>124</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="13">
         <v>858.76</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18">
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13">
         <v>1</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="13">
         <v>64</v>
       </c>
-      <c r="J10" s="18">
+      <c r="J10" s="13">
         <v>575.36</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="13">
         <v>2</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="13">
         <v>78</v>
       </c>
-      <c r="M10" s="18">
+      <c r="M10" s="13">
         <v>565.22</v>
       </c>
-      <c r="N10" s="18">
+      <c r="N10" s="13">
         <v>2</v>
       </c>
-      <c r="O10" s="18">
+      <c r="O10" s="13">
         <v>130</v>
       </c>
-      <c r="P10" s="18">
+      <c r="P10" s="13">
         <v>363.70000000000005</v>
       </c>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18">
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13">
         <v>8</v>
       </c>
-      <c r="U10" s="18">
+      <c r="U10" s="13">
         <v>396</v>
       </c>
-      <c r="V10" s="18">
+      <c r="V10" s="13">
         <v>2363.04</v>
       </c>
     </row>
@@ -6410,49 +6477,49 @@
       <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="13">
         <v>1</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="13">
         <v>50</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="13">
         <v>999.49999999999989</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="13">
         <v>1</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="13">
         <v>5</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="13">
         <v>625</v>
       </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18">
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13">
         <v>2</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="13">
         <v>138</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="13">
         <v>1484.94</v>
       </c>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18">
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13">
         <v>4</v>
       </c>
-      <c r="U11" s="18">
+      <c r="U11" s="13">
         <v>193</v>
       </c>
-      <c r="V11" s="18">
+      <c r="V11" s="13">
         <v>3109.44</v>
       </c>
     </row>
@@ -6460,49 +6527,49 @@
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="13">
         <v>1</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="13">
         <v>28</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="13">
         <v>251.72</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18">
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13">
         <v>1</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="13">
         <v>55</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="13">
         <v>686.95</v>
       </c>
-      <c r="N12" s="18">
+      <c r="N12" s="13">
         <v>1</v>
       </c>
-      <c r="O12" s="18">
+      <c r="O12" s="13">
         <v>90</v>
       </c>
-      <c r="P12" s="18">
+      <c r="P12" s="13">
         <v>449.1</v>
       </c>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18">
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13">
         <v>3</v>
       </c>
-      <c r="U12" s="18">
+      <c r="U12" s="13">
         <v>173</v>
       </c>
-      <c r="V12" s="18">
+      <c r="V12" s="13">
         <v>1387.77</v>
       </c>
     </row>
@@ -6510,49 +6577,49 @@
       <c r="A13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="13">
         <v>1</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="13">
         <v>81</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="13">
         <v>1619.1899999999998</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18">
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13">
         <v>1</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="13">
         <v>15</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="13">
         <v>299.84999999999997</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="13">
         <v>1</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="13">
         <v>74</v>
       </c>
-      <c r="M13" s="18">
+      <c r="M13" s="13">
         <v>1183.26</v>
       </c>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18">
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13">
         <v>3</v>
       </c>
-      <c r="U13" s="18">
+      <c r="U13" s="13">
         <v>170</v>
       </c>
-      <c r="V13" s="18">
+      <c r="V13" s="13">
         <v>3102.2999999999997</v>
       </c>
     </row>
@@ -6560,49 +6627,49 @@
       <c r="A14" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="13">
         <v>1</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="13">
         <v>87</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="13">
         <v>1305</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="13">
         <v>1</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="13">
         <v>2</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="13">
         <v>250</v>
       </c>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18">
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13">
         <v>1</v>
       </c>
-      <c r="O14" s="18">
+      <c r="O14" s="13">
         <v>67</v>
       </c>
-      <c r="P14" s="18">
+      <c r="P14" s="13">
         <v>86.43</v>
       </c>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18">
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13">
         <v>3</v>
       </c>
-      <c r="U14" s="18">
+      <c r="U14" s="13">
         <v>156</v>
       </c>
-      <c r="V14" s="18">
+      <c r="V14" s="13">
         <v>1641.43</v>
       </c>
     </row>
@@ -6610,55 +6677,55 @@
       <c r="A15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="13">
         <v>1</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="13">
         <v>7</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="13">
         <v>139.92999999999998</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="13">
         <v>1</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="13">
         <v>3</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="13">
         <v>825</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="13">
         <v>1</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="13">
         <v>76</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="13">
         <v>151.24</v>
       </c>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18">
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13">
         <v>1</v>
       </c>
-      <c r="O15" s="18">
+      <c r="O15" s="13">
         <v>56</v>
       </c>
-      <c r="P15" s="18">
+      <c r="P15" s="13">
         <v>167.44</v>
       </c>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18">
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13">
         <v>4</v>
       </c>
-      <c r="U15" s="18">
+      <c r="U15" s="13">
         <v>142</v>
       </c>
-      <c r="V15" s="18">
+      <c r="V15" s="13">
         <v>1283.6100000000001</v>
       </c>
     </row>
@@ -6666,157 +6733,157 @@
       <c r="A16" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="13">
         <v>1</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="13">
         <v>57</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="13">
         <v>1139.4299999999998</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18">
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13">
         <v>1</v>
       </c>
-      <c r="O16" s="18">
+      <c r="O16" s="13">
         <v>32</v>
       </c>
-      <c r="P16" s="18">
+      <c r="P16" s="13">
         <v>63.68</v>
       </c>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18">
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13">
         <v>2</v>
       </c>
-      <c r="U16" s="18">
+      <c r="U16" s="13">
         <v>89</v>
       </c>
-      <c r="V16" s="18">
+      <c r="V16" s="13">
         <v>1203.1099999999999</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
+        <v>41</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
     </row>
     <row r="18" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="13">
         <v>15</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="13">
         <v>722</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="13">
         <v>9577.6500000000015</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="13">
         <v>3</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="13">
         <v>10</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="13">
         <v>1700</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="13">
         <v>5</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="13">
         <v>278</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="13">
         <v>2045.22</v>
       </c>
-      <c r="K18" s="18">
+      <c r="K18" s="13">
         <v>7</v>
       </c>
-      <c r="L18" s="18">
+      <c r="L18" s="13">
         <v>395</v>
       </c>
-      <c r="M18" s="18">
+      <c r="M18" s="13">
         <v>4169.87</v>
       </c>
-      <c r="N18" s="18">
+      <c r="N18" s="13">
         <v>13</v>
       </c>
-      <c r="O18" s="18">
+      <c r="O18" s="13">
         <v>716</v>
       </c>
-      <c r="P18" s="18">
+      <c r="P18" s="13">
         <v>2135.14</v>
       </c>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18">
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13">
         <v>43</v>
       </c>
-      <c r="U18" s="18">
+      <c r="U18" s="13">
         <v>2121</v>
       </c>
-      <c r="V18" s="18">
+      <c r="V18" s="13">
         <v>19627.88</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="18"/>
-      <c r="V19" s="18"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
     </row>
     <row r="20" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
@@ -6828,15 +6895,15 @@
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
-      <c r="N20" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="37"/>
-      <c r="T20" s="38"/>
+      <c r="N20" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="O20" s="33"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="33"/>
+      <c r="R20" s="33"/>
+      <c r="S20" s="33"/>
+      <c r="T20" s="34"/>
     </row>
     <row r="21" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
@@ -6854,15 +6921,15 @@
       <c r="E21" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="N21" s="39" t="s">
+      <c r="N21" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="O21" s="40"/>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="40"/>
-      <c r="R21" s="40"/>
-      <c r="S21" s="40"/>
-      <c r="T21" s="41"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="37"/>
     </row>
     <row r="22" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
@@ -6880,15 +6947,15 @@
       <c r="E22" s="13">
         <v>15</v>
       </c>
-      <c r="N22" s="39" t="s">
+      <c r="N22" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="O22" s="40"/>
-      <c r="P22" s="40"/>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="40"/>
-      <c r="S22" s="40"/>
-      <c r="T22" s="41"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="37"/>
     </row>
     <row r="23" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
@@ -6904,15 +6971,15 @@
       <c r="E23" s="13">
         <v>3</v>
       </c>
-      <c r="N23" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="O23" s="43"/>
-      <c r="P23" s="43"/>
-      <c r="Q23" s="43"/>
-      <c r="R23" s="43"/>
-      <c r="S23" s="43"/>
-      <c r="T23" s="44"/>
+      <c r="N23" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="O23" s="40"/>
+      <c r="P23" s="40"/>
+      <c r="Q23" s="40"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="40"/>
+      <c r="T23" s="41"/>
     </row>
     <row r="24" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
@@ -6931,7 +6998,7 @@
         <v>5</v>
       </c>
       <c r="N24" s="39" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="O24" s="40"/>
       <c r="P24" s="40"/>
@@ -6940,7 +7007,7 @@
       <c r="S24" s="40"/>
       <c r="T24" s="41"/>
     </row>
-    <row r="25" spans="1:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>21</v>
       </c>
@@ -6954,19 +7021,21 @@
       <c r="E25" s="13">
         <v>7</v>
       </c>
-      <c r="J25" s="33" t="s">
+      <c r="J25" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="K25" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="N25" s="45"/>
-      <c r="O25" s="46"/>
-      <c r="P25" s="46"/>
-      <c r="Q25" s="46"/>
-      <c r="R25" s="46"/>
-      <c r="S25" s="46"/>
-      <c r="T25" s="47"/>
+      <c r="K25" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="N25" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="40"/>
+      <c r="R25" s="40"/>
+      <c r="S25" s="40"/>
+      <c r="T25" s="41"/>
     </row>
     <row r="26" spans="1:22" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
@@ -6984,10 +7053,19 @@
       <c r="E26" s="13">
         <v>13</v>
       </c>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-    </row>
-    <row r="27" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="N26" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="O26" s="40"/>
+      <c r="P26" s="40"/>
+      <c r="Q26" s="40"/>
+      <c r="R26" s="40"/>
+      <c r="S26" s="40"/>
+      <c r="T26" s="41"/>
+    </row>
+    <row r="27" spans="1:22" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
         <v>27</v>
       </c>
@@ -7003,20 +7081,27 @@
       <c r="E27" s="13">
         <v>43</v>
       </c>
-      <c r="J27" s="33" t="s">
+      <c r="J27" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="K27" s="34" t="s">
+      <c r="K27" s="31" t="s">
         <v>34</v>
       </c>
       <c r="L27" s="17"/>
       <c r="M27" s="17"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="42"/>
+      <c r="Q27" s="42"/>
+      <c r="R27" s="42"/>
+      <c r="S27" s="42"/>
+      <c r="T27" s="43"/>
     </row>
     <row r="28" spans="1:22" ht="18" x14ac:dyDescent="0.2">
-      <c r="J28" s="34" t="s">
+      <c r="J28" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="K28" s="35">
+      <c r="K28" s="31">
         <v>15</v>
       </c>
       <c r="L28" s="17"/>
@@ -7034,10 +7119,10 @@
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
-      <c r="J29" s="34" t="s">
+      <c r="J29" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="K29" s="35">
+      <c r="K29" s="31">
         <v>3</v>
       </c>
     </row>
@@ -7063,10 +7148,10 @@
       <c r="G30" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J30" s="34" t="s">
+      <c r="J30" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="K30" s="35">
+      <c r="K30" s="31">
         <v>5</v>
       </c>
     </row>
@@ -7074,28 +7159,28 @@
       <c r="A31" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="13">
+      <c r="B31" s="44">
         <v>8</v>
       </c>
-      <c r="C31" s="13">
+      <c r="C31" s="44">
         <v>2</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="44">
         <v>1</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="44">
         <v>4</v>
       </c>
-      <c r="F31" s="13">
+      <c r="F31" s="44">
         <v>9</v>
       </c>
-      <c r="G31" s="13">
+      <c r="G31" s="44">
         <v>24</v>
       </c>
-      <c r="J31" s="34" t="s">
+      <c r="J31" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="K31" s="35">
+      <c r="K31" s="31">
         <v>7</v>
       </c>
     </row>
@@ -7103,26 +7188,26 @@
       <c r="A32" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="13">
+      <c r="B32" s="44">
         <v>5</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13">
+      <c r="C32" s="44"/>
+      <c r="D32" s="44">
         <v>3</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="44">
         <v>3</v>
       </c>
-      <c r="F32" s="13">
+      <c r="F32" s="44">
         <v>2</v>
       </c>
-      <c r="G32" s="13">
+      <c r="G32" s="44">
         <v>13</v>
       </c>
-      <c r="J32" s="34" t="s">
+      <c r="J32" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="K32" s="35">
+      <c r="K32" s="31">
         <v>13</v>
       </c>
     </row>
@@ -7130,26 +7215,26 @@
       <c r="A33" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="13">
+      <c r="B33" s="44">
         <v>2</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="44">
         <v>1</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33" s="44">
         <v>1</v>
       </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13">
+      <c r="E33" s="44"/>
+      <c r="F33" s="44">
         <v>2</v>
       </c>
-      <c r="G33" s="13">
+      <c r="G33" s="44">
         <v>6</v>
       </c>
-      <c r="J33" s="34" t="s">
+      <c r="J33" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="K33" s="35">
+      <c r="K33" s="31">
         <v>43</v>
       </c>
     </row>
@@ -7157,41 +7242,39 @@
       <c r="A34" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="13">
+      <c r="B34" s="44">
         <v>15</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="44">
         <v>3</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="44">
         <v>5</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="44">
         <v>7</v>
       </c>
-      <c r="F34" s="13">
+      <c r="F34" s="44">
         <v>13</v>
       </c>
-      <c r="G34" s="13">
+      <c r="G34" s="44">
         <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="21"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
     </row>
     <row r="36" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="J36" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="K36" s="23"/>
-      <c r="L36" s="23"/>
-      <c r="M36" s="23"/>
-      <c r="N36" s="24"/>
-      <c r="O36" s="24"/>
-      <c r="P36" s="25"/>
+      <c r="J36" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="22"/>
     </row>
     <row r="37" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
@@ -7200,15 +7283,15 @@
       <c r="B37" t="s">
         <v>28</v>
       </c>
-      <c r="J37" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="K37" s="27"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="27"/>
-      <c r="N37" s="28"/>
-      <c r="O37" s="28"/>
-      <c r="P37" s="29"/>
+      <c r="J37" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
+      <c r="N37" s="25"/>
+      <c r="O37" s="25"/>
+      <c r="P37" s="26"/>
     </row>
     <row r="38" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="14">
@@ -7217,13 +7300,13 @@
       <c r="B38" s="10">
         <v>1.99</v>
       </c>
-      <c r="J38" s="26"/>
-      <c r="K38" s="28"/>
-      <c r="L38" s="28"/>
-      <c r="M38" s="28"/>
-      <c r="N38" s="28"/>
-      <c r="O38" s="28"/>
-      <c r="P38" s="29"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="25"/>
+      <c r="M38" s="25"/>
+      <c r="N38" s="25"/>
+      <c r="O38" s="25"/>
+      <c r="P38" s="26"/>
     </row>
     <row r="39" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="14">
@@ -7232,15 +7315,15 @@
       <c r="B39" s="10">
         <v>19.989999999999998</v>
       </c>
-      <c r="J39" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="K39" s="28"/>
-      <c r="L39" s="28"/>
-      <c r="M39" s="28"/>
-      <c r="N39" s="28"/>
-      <c r="O39" s="28"/>
-      <c r="P39" s="29"/>
+      <c r="J39" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="25"/>
+      <c r="O39" s="25"/>
+      <c r="P39" s="26"/>
     </row>
     <row r="40" spans="1:16" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="14">
@@ -7249,15 +7332,15 @@
       <c r="B40" s="10">
         <v>4.99</v>
       </c>
-      <c r="J40" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="28"/>
-      <c r="N40" s="28"/>
-      <c r="O40" s="28"/>
-      <c r="P40" s="29"/>
+      <c r="J40" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="K40" s="25"/>
+      <c r="L40" s="25"/>
+      <c r="M40" s="25"/>
+      <c r="N40" s="25"/>
+      <c r="O40" s="25"/>
+      <c r="P40" s="26"/>
     </row>
     <row r="41" spans="1:16" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
@@ -7266,15 +7349,15 @@
       <c r="B41" s="10">
         <v>19.989999999999998</v>
       </c>
-      <c r="J41" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="K41" s="31"/>
-      <c r="L41" s="31"/>
-      <c r="M41" s="31"/>
-      <c r="N41" s="31"/>
-      <c r="O41" s="31"/>
-      <c r="P41" s="32"/>
+      <c r="J41" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="K41" s="28"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="28"/>
+      <c r="N41" s="28"/>
+      <c r="O41" s="28"/>
+      <c r="P41" s="29"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="14">
@@ -7597,6 +7680,12 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="N23:T23"/>
+    <mergeCell ref="N24:T24"/>
+    <mergeCell ref="N26:T26"/>
+    <mergeCell ref="N25:T25"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -7634,7 +7723,7 @@
       <c r="A4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="17">
         <v>8</v>
       </c>
     </row>
@@ -7642,7 +7731,7 @@
       <c r="A5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="17">
         <v>2</v>
       </c>
     </row>
@@ -7650,7 +7739,7 @@
       <c r="A6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="17">
         <v>1</v>
       </c>
     </row>
@@ -7658,7 +7747,7 @@
       <c r="A7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="17">
         <v>4</v>
       </c>
     </row>
@@ -7666,7 +7755,7 @@
       <c r="A8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="17">
         <v>9</v>
       </c>
     </row>
@@ -7674,7 +7763,7 @@
       <c r="A9" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="17">
         <v>24</v>
       </c>
     </row>
@@ -7715,7 +7804,7 @@
       <c r="A4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="17">
         <v>5</v>
       </c>
     </row>
@@ -7723,7 +7812,7 @@
       <c r="A5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="17">
         <v>3</v>
       </c>
     </row>
@@ -7731,7 +7820,7 @@
       <c r="A6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="17">
         <v>3</v>
       </c>
     </row>
@@ -7739,7 +7828,7 @@
       <c r="A7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="17">
         <v>2</v>
       </c>
     </row>
@@ -7747,7 +7836,7 @@
       <c r="A8" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="17">
         <v>13</v>
       </c>
     </row>
@@ -7788,7 +7877,7 @@
       <c r="A4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="17">
         <v>2</v>
       </c>
     </row>
@@ -7796,7 +7885,7 @@
       <c r="A5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="17">
         <v>1</v>
       </c>
     </row>
@@ -7804,7 +7893,7 @@
       <c r="A6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="17">
         <v>1</v>
       </c>
     </row>
@@ -7812,7 +7901,7 @@
       <c r="A7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="17">
         <v>2</v>
       </c>
     </row>
@@ -7820,7 +7909,7 @@
       <c r="A8" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="17">
         <v>6</v>
       </c>
     </row>

</xml_diff>